<commit_message>
new dashboard and files
</commit_message>
<xml_diff>
--- a/public/risk_threshold.xlsx
+++ b/public/risk_threshold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PhpstormProjects\wiat_front\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20FC915-457F-4E50-8E42-559F316ECC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D7142E3-BE8F-41EA-A6A6-498AD6E48977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{C8DB30FF-034D-4F5E-A8CE-87B2AA9556C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Low</t>
   </si>
@@ -49,7 +49,7 @@
   </si>
   <si>
     <r>
-      <t>Recycled water factor</t>
+      <t>Dilution factor</t>
     </r>
     <r>
       <rPr>
@@ -66,7 +66,7 @@
   </si>
   <si>
     <r>
-      <t>Dilution factor</t>
+      <t>Consumption available ratio</t>
     </r>
     <r>
       <rPr>
@@ -78,12 +78,126 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Increase in the concentration of the pollutant in the receiving body</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Increase in toxic units in the receiving water body after discharge</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Carbon impact</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Toxic units in the effluent</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; Higher values means higher impacts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Treated water factor</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; Higher values means lower impacts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Concentration of the effluent pollutants (with respect to EQS)</t>
     </r>
     <r>
       <rPr>
@@ -95,12 +209,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Consumption available ratio</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Increase of the concentration of the effluent pollutants in the receiving water body after discharge (with respect to EQS)</t>
     </r>
     <r>
       <rPr>
@@ -117,28 +231,12 @@
   </si>
   <si>
     <r>
-      <t>Specific water consumption</t>
+      <t>Eutrophication potential</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Eutrophication potential</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+        <u/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -147,171 +245,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Increase in the concentration of the pollutant in the receiving body</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Increase in toxic units in the receiving water body after discharge</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Average concentration of the effluent pollutants (with respect to EQS)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Increase of the average concentration of the effluent pollutants in the receiving water body after discharge (with respect to EQS)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Percentage of treatment efficiency (compared to WWTP influent)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Carbon impact</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Toxic units in the effluent</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> --&gt; Higher values means higher impacts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> --&gt; Higher values means lower impacts</t>
     </r>
   </si>
 </sst>
@@ -319,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +286,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,6 +375,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,11 +690,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131E30A0-4211-4C5A-8B5B-19CA9E80E21E}">
-  <dimension ref="A3:F35"/>
+  <dimension ref="A3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -764,7 +715,7 @@
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -788,29 +739,29 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -818,8 +769,8 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+      <c r="A10" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -827,79 +778,44 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
+      <c r="A11" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
+      <c r="A17" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>